<commit_message>
Edited excel file. Simplified instructions.
</commit_message>
<xml_diff>
--- a/docs/unit3/05_python_and_excel/data.xlsx
+++ b/docs/unit3/05_python_and_excel/data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/Library/CloudStorage/GoogleDrive-njones61@gmail.com/.shortcut-targets-by-id/13JXjAERDUolONfwbHdYJ6lqWydrgdQN6/CCE 270 Fall 2024/Unit 3/5. Python plus Excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0088E9-DCBE-9940-833B-23E86A9BEF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="9975"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="23000" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>GDP</t>
   </si>
@@ -29,11 +35,14 @@
   <si>
     <t>G</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -76,14 +85,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -121,7 +133,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -193,7 +205,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -366,16 +378,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -389,7 +404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>29281</v>
       </c>
@@ -406,7 +421,7 @@
         <v>1365.4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>29373</v>
       </c>
@@ -423,7 +438,7 @@
         <v>1369.7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>29465</v>
       </c>
@@ -440,7 +455,7 @@
         <v>1350.8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>29556</v>
       </c>
@@ -457,7 +472,7 @@
         <v>1349.4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>29646</v>
       </c>
@@ -474,7 +489,7 @@
         <v>1367.3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>29738</v>
       </c>
@@ -491,7 +506,7 @@
         <v>1370.4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>29830</v>
       </c>
@@ -508,7 +523,7 @@
         <v>1367.3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>29921</v>
       </c>
@@ -525,7 +540,7 @@
         <v>1379.9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>30011</v>
       </c>
@@ -542,7 +557,7 @@
         <v>1378.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>30103</v>
       </c>
@@ -559,7 +574,7 @@
         <v>1386.5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>30195</v>
       </c>
@@ -576,7 +591,7 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>30286</v>
       </c>
@@ -593,7 +608,7 @@
         <v>1420.1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>30376</v>
       </c>
@@ -610,7 +625,7 @@
         <v>1430.8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>30468</v>
       </c>
@@ -627,7 +642,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>30560</v>
       </c>
@@ -644,7 +659,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>30651</v>
       </c>
@@ -661,7 +676,7 @@
         <v>1443.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>30742</v>
       </c>
@@ -678,7 +693,7 @@
         <v>1457.8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>30834</v>
       </c>
@@ -695,7 +710,7 @@
         <v>1489.2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>30926</v>
       </c>
@@ -712,7 +727,7 @@
         <v>1500.2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>31017</v>
       </c>
@@ -729,7 +744,7 @@
         <v>1532.3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>31107</v>
       </c>
@@ -746,7 +761,7 @@
         <v>1549.9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>31199</v>
       </c>
@@ -763,7 +778,7 @@
         <v>1584.7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>31291</v>
       </c>
@@ -780,7 +795,7 @@
         <v>1625.8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>31382</v>
       </c>
@@ -797,7 +812,7 @@
         <v>1635.5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>31472</v>
       </c>
@@ -814,7 +829,7 @@
         <v>1653.2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>31564</v>
       </c>
@@ -831,7 +846,7 @@
         <v>1688.3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>31656</v>
       </c>
@@ -848,7 +863,7 @@
         <v>1726.6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>31747</v>
       </c>
@@ -865,7 +880,7 @@
         <v>1716.6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>31837</v>
       </c>
@@ -882,7 +897,7 @@
         <v>1723.7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>31929</v>
       </c>
@@ -899,7 +914,7 @@
         <v>1734.6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>32021</v>
       </c>
@@ -916,7 +931,7 @@
         <v>1734.6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32112</v>
       </c>
@@ -933,7 +948,7 @@
         <v>1755.6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32203</v>
       </c>
@@ -950,7 +965,7 @@
         <v>1747.1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>32295</v>
       </c>
@@ -967,7 +982,7 @@
         <v>1751.7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>32387</v>
       </c>
@@ -984,7 +999,7 @@
         <v>1750.7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>32478</v>
       </c>
@@ -1001,7 +1016,7 @@
         <v>1786.2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>32568</v>
       </c>
@@ -1018,7 +1033,7 @@
         <v>1775.2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>32660</v>
       </c>
@@ -1035,7 +1050,7 @@
         <v>1802.8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>32752</v>
       </c>
@@ -1052,7 +1067,7 @@
         <v>1819.7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>32843</v>
       </c>
@@ -1069,7 +1084,7 @@
         <v>1829.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>32933</v>
       </c>
@@ -1086,7 +1101,7 @@
         <v>1857.6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>33025</v>
       </c>
@@ -1103,7 +1118,7 @@
         <v>1860.4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>33117</v>
       </c>
@@ -1120,7 +1135,7 @@
         <v>1859.8</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>33208</v>
       </c>
@@ -1137,7 +1152,7 @@
         <v>1878.3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>33298</v>
       </c>
@@ -1154,7 +1169,7 @@
         <v>1885.9</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>33390</v>
       </c>
@@ -1171,7 +1186,7 @@
         <v>1892.5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>33482</v>
       </c>
@@ -1188,7 +1203,7 @@
         <v>1883.5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>33573</v>
       </c>
@@ -1205,7 +1220,7 @@
         <v>1875.6</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>33664</v>
       </c>
@@ -1222,7 +1237,7 @@
         <v>1889.9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>33756</v>
       </c>
@@ -1239,7 +1254,7 @@
         <v>1887.6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>33848</v>
       </c>
@@ -1256,7 +1271,7 @@
         <v>1897.3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>33939</v>
       </c>
@@ -1273,7 +1288,7 @@
         <v>1897.9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>34029</v>
       </c>
@@ -1290,7 +1305,7 @@
         <v>1877.9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>34121</v>
       </c>
@@ -1307,7 +1322,7 @@
         <v>1876.5</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>34213</v>
       </c>
@@ -1324,7 +1339,7 @@
         <v>1874.6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>34304</v>
       </c>
@@ -1341,7 +1356,7 @@
         <v>1883.9</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>34394</v>
       </c>
@@ -1358,7 +1373,7 @@
         <v>1859.9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>34486</v>
       </c>
@@ -1375,7 +1390,7 @@
         <v>1867.7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>34578</v>
       </c>
@@ -1392,7 +1407,7 @@
         <v>1900.5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>34669</v>
       </c>
@@ -1409,7 +1424,7 @@
         <v>1884.1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>34759</v>
       </c>
@@ -1426,7 +1441,7 @@
         <v>1891.6</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>34851</v>
       </c>
@@ -1443,7 +1458,7 @@
         <v>1897.9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>34943</v>
       </c>
@@ -1460,7 +1475,7 @@
         <v>1893.7</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>35034</v>
       </c>
@@ -1477,7 +1492,7 @@
         <v>1872.5</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>35125</v>
       </c>
@@ -1494,7 +1509,7 @@
         <v>1884.5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>35217</v>
       </c>
@@ -1511,7 +1526,7 @@
         <v>1911.6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>35309</v>
       </c>
@@ -1528,7 +1543,7 @@
         <v>1909.7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>35400</v>
       </c>
@@ -1545,7 +1560,7 @@
         <v>1925.9</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>35490</v>
       </c>
@@ -1562,7 +1577,7 @@
         <v>1929.4</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>35582</v>
       </c>
@@ -1579,7 +1594,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>35674</v>
       </c>
@@ -1596,7 +1611,7 @@
         <v>1948.2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>35765</v>
       </c>
@@ -1613,7 +1628,7 @@
         <v>1951.5</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>35855</v>
       </c>
@@ -1630,7 +1645,7 @@
         <v>1939.7</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>35947</v>
       </c>
@@ -1647,7 +1662,7 @@
         <v>1981.9</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>36039</v>
       </c>
@@ -1664,7 +1679,7 @@
         <v>2000.2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>36130</v>
       </c>
@@ -1681,7 +1696,7 @@
         <v>2018.1</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>36220</v>
       </c>
@@ -1698,7 +1713,7 @@
         <v>2028.4</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>36312</v>
       </c>
@@ -1715,7 +1730,7 @@
         <v>2036.9</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>36404</v>
       </c>
@@ -1732,7 +1747,7 @@
         <v>2063.3000000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>36495</v>
       </c>
@@ -1749,7 +1764,7 @@
         <v>2095.9</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>36586</v>
       </c>
@@ -1766,7 +1781,7 @@
         <v>2078.6999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>36678</v>
       </c>
@@ -1783,7 +1798,7 @@
         <v>2106.4</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>36770</v>
       </c>
@@ -1800,7 +1815,7 @@
         <v>2099.8000000000002</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>36861</v>
       </c>
@@ -1817,7 +1832,7 @@
         <v>2106.1999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>36951</v>
       </c>
@@ -1834,7 +1849,7 @@
         <v>2137.3000000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>37043</v>
       </c>
@@ -1851,7 +1866,7 @@
         <v>2181.6999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>37135</v>
       </c>
@@ -1868,7 +1883,7 @@
         <v>2177.8000000000002</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>37226</v>
       </c>
@@ -1885,7 +1900,7 @@
         <v>2216.4</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>37316</v>
       </c>
@@ -1902,7 +1917,7 @@
         <v>2250.4</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>37408</v>
       </c>
@@ -1919,7 +1934,7 @@
         <v>2272</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>37500</v>
       </c>
@@ -1936,7 +1951,7 @@
         <v>2290.4</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>37591</v>
       </c>
@@ -1953,7 +1968,7 @@
         <v>2305.6999999999998</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>37681</v>
       </c>
@@ -1970,7 +1985,7 @@
         <v>2300.9</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>37773</v>
       </c>
@@ -1987,7 +2002,7 @@
         <v>2335.1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>37865</v>
       </c>
@@ -2004,7 +2019,7 @@
         <v>2342</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>37956</v>
       </c>
@@ -2021,7 +2036,7 @@
         <v>2343.6999999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>38047</v>
       </c>
@@ -2038,7 +2053,7 @@
         <v>2354.9</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>38139</v>
       </c>
@@ -2055,7 +2070,7 @@
         <v>2363.5</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>38231</v>
       </c>
@@ -2072,7 +2087,7 @@
         <v>2372.1</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>38322</v>
       </c>
@@ -2089,7 +2104,7 @@
         <v>2357.6</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>38412</v>
       </c>
@@ -2106,7 +2121,7 @@
         <v>2359.9</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>38504</v>
       </c>
@@ -2123,7 +2138,7 @@
         <v>2362.4</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>38596</v>
       </c>
@@ -2140,7 +2155,7 @@
         <v>2383.9</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>38687</v>
       </c>
@@ -2157,7 +2172,7 @@
         <v>2373.4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>38777</v>
       </c>
@@ -2174,7 +2189,7 @@
         <v>2397.1</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>38869</v>
       </c>
@@ -2191,7 +2206,7 @@
         <v>2399.1</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>38961</v>
       </c>
@@ -2208,7 +2223,7 @@
         <v>2402.6999999999998</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>39052</v>
       </c>
@@ -2225,7 +2240,7 @@
         <v>2409.4</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>39142</v>
       </c>
@@ -2242,7 +2257,7 @@
         <v>2406.6999999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>39234</v>
       </c>
@@ -2259,7 +2274,7 @@
         <v>2426.8000000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>39326</v>
       </c>
@@ -2276,7 +2291,7 @@
         <v>2447.9</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>39417</v>
       </c>
@@ -2293,7 +2308,7 @@
         <v>2455.3000000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>39508</v>
       </c>
@@ -2310,7 +2325,7 @@
         <v>2473.9</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>39600</v>
       </c>
@@ -2327,7 +2342,7 @@
         <v>2484.5</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>39692</v>
       </c>
@@ -2344,7 +2359,7 @@
         <v>2510.6999999999998</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>39783</v>
       </c>
@@ -2361,7 +2376,7 @@
         <v>2520.5</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>39873</v>
       </c>
@@ -2378,7 +2393,7 @@
         <v>2509.6</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>39965</v>
       </c>
@@ -2395,7 +2410,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>40057</v>
       </c>
@@ -2412,7 +2427,7 @@
         <v>2554.1999999999998</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>40148</v>
       </c>
@@ -2429,7 +2444,7 @@
         <v>2548.5</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>40238</v>
       </c>
@@ -2446,7 +2461,7 @@
         <v>2540.6</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>40330</v>
       </c>
@@ -2463,7 +2478,7 @@
         <v>2564</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>40422</v>
       </c>
@@ -2480,7 +2495,7 @@
         <v>2570.3000000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>40513</v>
       </c>
@@ -2497,7 +2512,7 @@
         <v>2552.1</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>40603</v>
       </c>
@@ -2514,7 +2529,7 @@
         <v>2513.9</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>40695</v>
       </c>
@@ -2531,7 +2546,7 @@
         <v>2508.1999999999998</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>40787</v>
       </c>
@@ -2548,7 +2563,7 @@
         <v>2507.6</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>40878</v>
       </c>
@@ -2565,7 +2580,7 @@
         <v>2481.1999999999998</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>40969</v>
       </c>
@@ -2588,24 +2603,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>